<commit_message>
Files added from 13-02-2024 upto 21-02-2024
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,33 @@
   </si>
   <si>
     <t>Functions and Arrays</t>
+  </si>
+  <si>
+    <t>Media Query</t>
+  </si>
+  <si>
+    <t>Transform, Transition, Animation</t>
+  </si>
+  <si>
+    <t>Flex, Grid</t>
+  </si>
+  <si>
+    <t>:root</t>
+  </si>
+  <si>
+    <t>GIT</t>
+  </si>
+  <si>
+    <t>Git installation, GitHub Overview</t>
+  </si>
+  <si>
+    <t>Datatypes, Operators, DOM Overview</t>
+  </si>
+  <si>
+    <t>Loops: while, for, do-while; various types of functions</t>
+  </si>
+  <si>
+    <t>Function, Array methods &amp; properties</t>
   </si>
 </sst>
 </file>
@@ -571,7 +598,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +874,9 @@
       <c r="D17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -860,7 +889,9 @@
       <c r="D18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
@@ -873,7 +904,9 @@
       <c r="D19" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
@@ -886,7 +919,9 @@
       <c r="D20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
@@ -899,7 +934,9 @@
       <c r="D21" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
@@ -925,7 +962,9 @@
       <c r="D23" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
@@ -938,18 +977,24 @@
       <c r="D24" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="6">
         <v>45343</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>

</xml_diff>

<commit_message>
Date: 22/24/26-02-2024 (Object files updated & DOM Introduction)
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>Class Status</t>
   </si>
@@ -183,10 +183,28 @@
     <t>Objects and Events</t>
   </si>
   <si>
-    <t>Objects</t>
-  </si>
-  <si>
     <t>[PROJECT] - Micro Project 2</t>
+  </si>
+  <si>
+    <t>Objects, Iterate through Objects, Nested Objects, Time Events</t>
+  </si>
+  <si>
+    <t>Understanding DOM</t>
+  </si>
+  <si>
+    <t>Closures + lev, var and cons</t>
+  </si>
+  <si>
+    <t>Micro Project 1 - Solution</t>
+  </si>
+  <si>
+    <t>DOM, Event Handling, Event Propogation, strict, pop-ups</t>
+  </si>
+  <si>
+    <t>let, var, const, self invoking function, closure</t>
+  </si>
+  <si>
+    <t>Constructors &amp; Prototypes</t>
   </si>
 </sst>
 </file>
@@ -215,7 +233,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,8 +293,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -314,11 +344,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -371,6 +455,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -680,8 +782,8 @@
   </sheetPr>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,13 +1230,13 @@
         <v>52</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1142,61 +1244,75 @@
         <v>45345</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="6">
         <v>45346</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="6">
         <v>45347</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="6">
         <v>45348</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="D30" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>59</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="6">
         <v>45349</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="D31" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="24"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
@@ -1209,7 +1325,7 @@
         <v>45350</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
@@ -1488,5 +1604,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
this keyword, constructor, call, apply, bind,  prototype, class
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>Class Status</t>
   </si>
@@ -201,17 +201,37 @@
     <t>DOM, Event Handling, Event Propogation, strict, pop-ups</t>
   </si>
   <si>
-    <t>let, var, const, self invoking function, closure</t>
-  </si>
-  <si>
     <t>Constructors &amp; Prototypes</t>
+  </si>
+  <si>
+    <t>Prototypes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">let, var, const, self invoking function, closure, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Arrow Function</t>
+    </r>
+  </si>
+  <si>
+    <t>this keyword, constuctor function, call, apply, bind</t>
+  </si>
+  <si>
+    <t>prototype, class</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +249,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -402,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -473,6 +499,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -782,8 +811,8 @@
   </sheetPr>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1124,7 @@
       <c r="D18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="26" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="3"/>
@@ -1296,7 +1325,7 @@
         <v>56</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1310,22 +1339,28 @@
         <v>45349</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="24"/>
+        <v>59</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>62</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="6">
         <v>45350</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="23"/>
+      <c r="D32" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>

</xml_diff>

<commit_message>
Promise, Promise Chaining, Fetch, JQuery
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>Class Status</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t>prototype, class</t>
+  </si>
+  <si>
+    <t>promise, promise chaning, fetch</t>
+  </si>
+  <si>
+    <t>jquery introduction</t>
+  </si>
+  <si>
+    <t>jQuery</t>
+  </si>
+  <si>
+    <t>Promises</t>
   </si>
 </sst>
 </file>
@@ -812,7 +824,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,28 +1377,36 @@
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="6">
         <v>45351</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="D33" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="6">
         <v>45352</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="D34" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>

</xml_diff>

<commit_message>
Promise with setTimeout, Promise Chaining, Fetch Example
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>Class Status</t>
   </si>
@@ -207,11 +207,43 @@
     <t>Prototypes</t>
   </si>
   <si>
+    <t>this keyword, constuctor function, call, apply, bind</t>
+  </si>
+  <si>
+    <t>prototype, class</t>
+  </si>
+  <si>
+    <t>promise, promise chaning, fetch</t>
+  </si>
+  <si>
+    <t>jQuery</t>
+  </si>
+  <si>
+    <t>Promises</t>
+  </si>
+  <si>
+    <t>[PROJECT] - Micro Project 2 - Solution</t>
+  </si>
+  <si>
+    <t>Micro Project 2 - Solution</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">let, var, const, self invoking function, closure, </t>
+      <t>let, var, const, self invoking function, closure,</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Calibri"/>
@@ -221,29 +253,14 @@
     </r>
   </si>
   <si>
-    <t>this keyword, constuctor function, call, apply, bind</t>
-  </si>
-  <si>
-    <t>prototype, class</t>
-  </si>
-  <si>
-    <t>promise, promise chaning, fetch</t>
-  </si>
-  <si>
-    <t>jquery introduction</t>
-  </si>
-  <si>
-    <t>jQuery</t>
-  </si>
-  <si>
-    <t>Promises</t>
+    <t>jQuery introduction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +282,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
@@ -440,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -514,6 +545,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -823,8 +857,8 @@
   </sheetPr>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,7 +972,7 @@
       <c r="F6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
@@ -1337,7 +1371,7 @@
         <v>56</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1354,7 +1388,7 @@
         <v>59</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1371,7 +1405,7 @@
         <v>60</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1385,10 +1419,10 @@
         <v>45351</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -1402,36 +1436,42 @@
         <v>45352</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="6">
         <v>45353</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="D35" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>67</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C36" s="6">
         <v>45354</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>

</xml_diff>

<commit_message>
async, await, try, catch, throw
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
   <si>
     <t>Class Status</t>
   </si>
@@ -254,6 +254,15 @@
   </si>
   <si>
     <t>jQuery introduction</t>
+  </si>
+  <si>
+    <t>async, await, try, catch, throw</t>
+  </si>
+  <si>
+    <t>Async and Await</t>
+  </si>
+  <si>
+    <t>[PROJECT] - Micro Project 3</t>
   </si>
 </sst>
 </file>
@@ -857,8 +866,8 @@
   </sheetPr>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,27 +1486,33 @@
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="6">
         <v>45355</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="6">
         <v>45356</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="19" t="s">
+        <v>72</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>

</xml_diff>

<commit_message>
26-03-2024: Introduction to React
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Cuvette MERN" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Cuvette MERN'!$A$1:$D$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cuvette MERN'!$A$1:$F$64</definedName>
   </definedNames>
   <calcPr calcId="52"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="87">
   <si>
     <t>Class Status</t>
   </si>
@@ -288,12 +288,30 @@
   <si>
     <t>React, node Installation, First Component Creation</t>
   </si>
+  <si>
+    <t>Displaying Data, Adding Styles, Conditional Rendering, Rendering Lists, Fragments</t>
+  </si>
+  <si>
+    <t>Props, Re-usable components using props, States intro using hooks, Event Handling</t>
+  </si>
+  <si>
+    <t>Forms (Controlled Components), Validations, Async state updates</t>
+  </si>
+  <si>
+    <t>Class Components</t>
+  </si>
+  <si>
+    <t>Component Life cycle and methods</t>
+  </si>
+  <si>
+    <t>Lifecycle Methods &amp; Uncontrolled Components</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,13 +351,6 @@
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -421,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -513,11 +524,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -627,7 +651,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -935,10 +971,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,7 +982,7 @@
     <col min="1" max="1" width="10.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.88671875" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
@@ -1885,7 +1921,7 @@
       <c r="E58" s="24"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="39"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="31" t="s">
         <v>7</v>
       </c>
@@ -1920,45 +1956,396 @@
       <c r="C61" s="32">
         <v>45379</v>
       </c>
-      <c r="D61" s="24"/>
+      <c r="D61" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="24"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="31" t="s">
         <v>16</v>
       </c>
       <c r="C62" s="32">
         <v>45380</v>
       </c>
-      <c r="D62" s="24"/>
+      <c r="D62" s="30" t="s">
+        <v>14</v>
+      </c>
       <c r="E62" s="24"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="28"/>
-      <c r="B63" s="31" t="s">
+      <c r="B63" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="32">
+      <c r="C63" s="40">
         <v>45381</v>
       </c>
       <c r="D63" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E63" s="24"/>
+      <c r="E63" s="41"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="24"/>
+      <c r="A64" s="42"/>
       <c r="B64" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C64" s="32">
         <v>45382</v>
       </c>
-      <c r="D64" s="24"/>
+      <c r="D64" s="43" t="s">
+        <v>14</v>
+      </c>
       <c r="E64" s="24"/>
     </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="24"/>
+      <c r="B65" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="32">
+        <v>45383</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" s="24"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="42"/>
+      <c r="B66" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="32">
+        <v>45384</v>
+      </c>
+      <c r="D66" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" s="24"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="24"/>
+      <c r="B67" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="32">
+        <v>45385</v>
+      </c>
+      <c r="D67" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E67" s="24"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="24"/>
+      <c r="B68" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="32">
+        <v>45386</v>
+      </c>
+      <c r="D68" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E68" s="24"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="24"/>
+      <c r="B69" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="32">
+        <v>45387</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E69" s="24"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="24"/>
+      <c r="B70" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="32">
+        <v>45388</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" s="24"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="28"/>
+      <c r="B71" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" s="32">
+        <v>45389</v>
+      </c>
+      <c r="D71" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71" s="24"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="24"/>
+      <c r="B72" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="32">
+        <v>45390</v>
+      </c>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="24"/>
+      <c r="B73" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="32">
+        <v>45391</v>
+      </c>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="24"/>
+      <c r="B74" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="32">
+        <v>45392</v>
+      </c>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="24"/>
+      <c r="B75" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="32">
+        <v>45393</v>
+      </c>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="24"/>
+      <c r="B76" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="32">
+        <v>45394</v>
+      </c>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="24"/>
+      <c r="B77" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="32">
+        <v>45395</v>
+      </c>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="24"/>
+      <c r="B78" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C78" s="32">
+        <v>45396</v>
+      </c>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="24"/>
+      <c r="B79" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="32">
+        <v>45397</v>
+      </c>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="24"/>
+      <c r="B80" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="32">
+        <v>45398</v>
+      </c>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="24"/>
+      <c r="B81" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="32">
+        <v>45399</v>
+      </c>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="24"/>
+      <c r="B82" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" s="32">
+        <v>45400</v>
+      </c>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="24"/>
+      <c r="B83" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83" s="32">
+        <v>45401</v>
+      </c>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="24"/>
+      <c r="B84" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="32">
+        <v>45402</v>
+      </c>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="24"/>
+      <c r="B85" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85" s="32">
+        <v>45403</v>
+      </c>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="24"/>
+      <c r="B86" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="32">
+        <v>45404</v>
+      </c>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="24"/>
+      <c r="B87" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="32">
+        <v>45405</v>
+      </c>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="24"/>
+      <c r="B88" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="32">
+        <v>45406</v>
+      </c>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="24"/>
+      <c r="B89" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="32">
+        <v>45407</v>
+      </c>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="24"/>
+      <c r="B90" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" s="32">
+        <v>45408</v>
+      </c>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="24"/>
+      <c r="B91" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="32">
+        <v>45409</v>
+      </c>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="24"/>
+      <c r="B92" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" s="32">
+        <v>45410</v>
+      </c>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="24"/>
+      <c r="B93" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="32">
+        <v>45411</v>
+      </c>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="24"/>
+      <c r="B94" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="32">
+        <v>45412</v>
+      </c>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F64"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Displaying Data, Adding Style, Fragments, Conditional Rendering, Rendering List
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -973,8 +973,8 @@
   </sheetPr>
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1921,7 +1921,7 @@
       <c r="E58" s="24"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="24"/>
+      <c r="A59" s="38"/>
       <c r="B59" s="31" t="s">
         <v>7</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="E60" s="24"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="24"/>
+      <c r="A61" s="38"/>
       <c r="B61" s="31" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
01-04-2024: Props, Re-usable components using props, States intro using hooks, Event Handling
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
   <si>
     <t>Class Status</t>
   </si>
@@ -295,16 +295,7 @@
     <t>Props, Re-usable components using props, States intro using hooks, Event Handling</t>
   </si>
   <si>
-    <t>Forms (Controlled Components), Validations, Async state updates</t>
-  </si>
-  <si>
-    <t>Class Components</t>
-  </si>
-  <si>
-    <t>Component Life cycle and methods</t>
-  </si>
-  <si>
-    <t>Lifecycle Methods &amp; Uncontrolled Components</t>
+    <t>Props, Re-use, States, Hooks(useState), Events</t>
   </si>
 </sst>
 </file>
@@ -973,8 +964,8 @@
   </sheetPr>
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,7 +1992,7 @@
       <c r="E64" s="24"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="24"/>
+      <c r="A65" s="38"/>
       <c r="B65" s="31" t="s">
         <v>5</v>
       </c>
@@ -2011,7 +2002,9 @@
       <c r="D65" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="E65" s="24"/>
+      <c r="E65" s="24" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="42"/>
@@ -2034,9 +2027,7 @@
       <c r="C67" s="32">
         <v>45385</v>
       </c>
-      <c r="D67" s="24" t="s">
-        <v>83</v>
-      </c>
+      <c r="D67" s="24"/>
       <c r="E67" s="24"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2047,9 +2038,7 @@
       <c r="C68" s="32">
         <v>45386</v>
       </c>
-      <c r="D68" s="24" t="s">
-        <v>84</v>
-      </c>
+      <c r="D68" s="24"/>
       <c r="E68" s="24"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2060,9 +2049,7 @@
       <c r="C69" s="32">
         <v>45387</v>
       </c>
-      <c r="D69" s="24" t="s">
-        <v>85</v>
-      </c>
+      <c r="D69" s="24"/>
       <c r="E69" s="24"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2073,9 +2060,7 @@
       <c r="C70" s="32">
         <v>45388</v>
       </c>
-      <c r="D70" s="24" t="s">
-        <v>86</v>
-      </c>
+      <c r="D70" s="24"/>
       <c r="E70" s="24"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
08-04-2024: Links added & Excel Sheet Update
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="107">
   <si>
     <t>Class Status</t>
   </si>
@@ -356,6 +356,15 @@
   </si>
   <si>
     <t>React Capstone Project Part 7</t>
+  </si>
+  <si>
+    <t>fetch data from api using fetch() &amp; .then() methods</t>
+  </si>
+  <si>
+    <t>moment, react-router-dom packages</t>
+  </si>
+  <si>
+    <t>styling and data rendering</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2015,7 +2024,9 @@
       <c r="D61" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="E61" s="24"/>
+      <c r="E61" s="24" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="27"/>
@@ -2164,7 +2175,9 @@
       <c r="D72" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="E72" s="24"/>
+      <c r="E72" s="24" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="43"/>
@@ -2177,7 +2190,9 @@
       <c r="D73" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="E73" s="24"/>
+      <c r="E73" s="24" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="41"/>

</xml_diff>

<commit_message>
12-06-2024: Initialise Capstone Frontend Project
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="134">
   <si>
     <t>Class Status</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>Backend Capstone Project Part 13</t>
+  </si>
+  <si>
+    <t>Created Controllers for Delete, Update Job and get filtered Jobs</t>
   </si>
 </sst>
 </file>
@@ -1129,8 +1132,8 @@
   </sheetPr>
   <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3067,7 +3070,9 @@
       <c r="D133" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="E133" s="24"/>
+      <c r="E133" s="24" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="41"/>

</xml_diff>